<commit_message>
commit service upload cer ,ws and add role
</commit_message>
<xml_diff>
--- a/workspace/back-end/ecert-webapp/src/main/resources/report/excel_template/RolePermission_Template.xlsx
+++ b/workspace/back-end/ecert-webapp/src/main/resources/report/excel_template/RolePermission_Template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wichien\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8AFA36-986D-42EC-8B8D-685CE73B4740}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="41">
   <si>
     <t xml:space="preserve">Role Name </t>
   </si>
@@ -154,12 +148,17 @@
   <si>
     <t>รายงาน Output VAT
 (UI-00009)</t>
+  </si>
+  <si>
+    <t>บันทึกข้อมูลจากเลขที่คำขอ 
+(TMB Req No.)
+(UI-00016)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -236,22 +235,22 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -317,7 +316,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -369,7 +368,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -563,424 +562,434 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AL3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AM5" sqref="AM5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.8" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="16.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.1796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7265625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.81640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.08984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" style="1" customWidth="1"/>
+    <col min="2" max="3" width="17.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.77734375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="13" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13.36328125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7265625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="38.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="38.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.453125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="36.44140625" style="1" customWidth="1"/>
     <col min="18" max="18" width="26" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.81640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="20.453125" style="1" customWidth="1"/>
-    <col min="21" max="21" width="14.36328125" style="1" customWidth="1"/>
-    <col min="22" max="22" width="22.453125" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.77734375" style="1" customWidth="1"/>
+    <col min="20" max="20" width="20.44140625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="14.33203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="22.44140625" style="1" customWidth="1"/>
     <col min="23" max="23" width="11" style="1" customWidth="1"/>
-    <col min="24" max="24" width="15.7265625" style="1" customWidth="1"/>
-    <col min="25" max="25" width="11.26953125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="10.90625" style="1" customWidth="1"/>
-    <col min="27" max="27" width="10.453125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7265625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="8.1796875" style="1" customWidth="1"/>
-    <col min="30" max="30" width="8.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.90625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="15.77734375" style="1" customWidth="1"/>
+    <col min="25" max="25" width="11.21875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="10.88671875" style="1" customWidth="1"/>
+    <col min="27" max="27" width="10.44140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="12.77734375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="8.21875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="8.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.88671875" style="1" customWidth="1"/>
     <col min="32" max="32" width="10" style="1" customWidth="1"/>
-    <col min="33" max="33" width="9.81640625" style="1" customWidth="1"/>
-    <col min="34" max="34" width="8.54296875" style="1" customWidth="1"/>
-    <col min="35" max="35" width="10.1796875" style="1" customWidth="1"/>
-    <col min="36" max="36" width="8.08984375" style="1" customWidth="1"/>
-    <col min="37" max="37" width="10.36328125" style="1" customWidth="1"/>
-    <col min="38" max="16384" width="8.7265625" style="1"/>
+    <col min="33" max="33" width="9.77734375" style="1" customWidth="1"/>
+    <col min="34" max="34" width="8.5546875" style="1" customWidth="1"/>
+    <col min="35" max="35" width="10.21875" style="1" customWidth="1"/>
+    <col min="36" max="36" width="8.109375" style="1" customWidth="1"/>
+    <col min="37" max="37" width="10.33203125" style="1" customWidth="1"/>
+    <col min="38" max="38" width="14.109375" style="1" customWidth="1"/>
+    <col min="39" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="45" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:38" ht="45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U1" s="2" t="s">
+      <c r="T1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="V1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="W1" s="2" t="s">
+      <c r="V1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="X1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="Y1" s="2" t="s">
+      <c r="X1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="Z1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AA1" s="2" t="s">
+      <c r="Z1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AB1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AB1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AD1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AD1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AH1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AI1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AI1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AK1" s="2" t="s">
-        <v>4</v>
+      <c r="AK1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="38.5" customHeight="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="8" t="s">
+    <row r="2" spans="1:38" ht="38.549999999999997" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="S2" s="8" t="s">
+      <c r="Q2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="U2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="V2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="W2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="X2" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Y2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Z2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AA2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AB2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="AC2" s="8" t="s">
+      <c r="AC2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AD2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AE2" s="8" t="s">
+      <c r="AE2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AF2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="AG2" s="8" t="s">
+      <c r="AG2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AH2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AI2" s="8" t="s">
+      <c r="AI2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AJ2" s="8" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AK2" s="8" t="s">
+      <c r="AK2" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="AL2" s="6" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:37" ht="18.5" x14ac:dyDescent="0.65">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:38" ht="18.600000000000001" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="V3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="W3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="X3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AI3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="AK3" s="5" t="s">
+      <c r="C3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL3" s="3" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:P1"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
     <mergeCell ref="Y1:Z1"/>
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="AC1:AG1"/>
     <mergeCell ref="AH1:AI1"/>
     <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:P1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" sqref="B3" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B3">
       <formula1>"Active,Inactive"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C3:AK3" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="C3:AL3">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fix bug role management
</commit_message>
<xml_diff>
--- a/workspace/back-end/ecert-webapp/src/main/resources/report/excel_template/RolePermission_Template.xlsx
+++ b/workspace/back-end/ecert-webapp/src/main/resources/report/excel_template/RolePermission_Template.xlsx
@@ -197,7 +197,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,6 +212,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,6 +262,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -265,10 +274,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -577,7 +583,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -587,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.21875" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.5"/>
@@ -600,21 +606,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="9" t="s">
+      <c r="B1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -622,10 +628,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -633,7 +639,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -644,7 +650,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -655,7 +661,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -666,7 +672,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -677,7 +683,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -688,7 +694,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -699,7 +705,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -710,7 +716,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -721,7 +727,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -732,7 +738,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="68.400000000000006" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -743,7 +749,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -754,7 +760,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -765,7 +771,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="23.4" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -776,10 +782,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -787,10 +793,10 @@
       </c>
     </row>
     <row r="18" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -798,10 +804,10 @@
       </c>
     </row>
     <row r="19" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -809,10 +815,10 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -820,10 +826,10 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -831,10 +837,10 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A22" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -842,7 +848,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="8" t="s">
         <v>36</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -853,7 +859,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -864,7 +870,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="8" t="s">
         <v>37</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -875,7 +881,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -886,7 +892,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="8" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -897,7 +903,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B28" s="10" t="s">
@@ -908,7 +914,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="8" t="s">
         <v>39</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -919,7 +925,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A30" s="7" t="s">
+      <c r="A30" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -930,7 +936,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -941,7 +947,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -952,7 +958,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A33" s="7" t="s">
+      <c r="A33" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="10" t="s">
@@ -963,7 +969,7 @@
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B34" s="10" t="s">
@@ -974,7 +980,7 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B35" s="10" t="s">
@@ -985,7 +991,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B36" s="10" t="s">
@@ -996,7 +1002,7 @@
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="8" t="s">
         <v>4</v>
       </c>
       <c r="B37" s="10" t="s">
@@ -1007,10 +1013,10 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1019,22 +1025,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B20"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="A23:A24"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="A29:A33"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B20"/>
-    <mergeCell ref="A21:B22"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A16"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" sqref="C2">

</xml_diff>